<commit_message>
Timber Testing program completed
</commit_message>
<xml_diff>
--- a/audio_database/Feature.xlsx
+++ b/audio_database/Feature.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit\Documents\MATLAB\Project\audio_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C068C964-DCA1-47B8-B8BC-2EFF3239E05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA102C2-11EB-42B3-8AC8-5F5E2989DECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{F98F55DE-6286-4433-92DF-1F34DB2F1572}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{F98F55DE-6286-4433-92DF-1F34DB2F1572}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -391,7 +391,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59FD446B-03FF-433F-A5A5-561D5C99261F}">
-  <dimension ref="A1:Z100"/>
+  <dimension ref="A1:AC100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:M75"/>
@@ -399,7 +399,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>5.0976174304885102</v>
       </c>
@@ -478,8 +478,17 @@
       <c r="Z1">
         <v>0.14247396748820057</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA1">
+        <v>7.5633522755776478E-2</v>
+      </c>
+      <c r="AB1">
+        <v>-1.2003473801069298E-2</v>
+      </c>
+      <c r="AC1">
+        <v>4.8442449559498203E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>6.2165876714931114</v>
       </c>
@@ -558,8 +567,17 @@
       <c r="Z2">
         <v>-0.1858613327163598</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA2">
+        <v>-5.150730329281162E-2</v>
+      </c>
+      <c r="AB2">
+        <v>6.3512861773581952E-2</v>
+      </c>
+      <c r="AC2">
+        <v>-5.5351821370128305E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4.315444665612219</v>
       </c>
@@ -638,8 +656,17 @@
       <c r="Z3">
         <v>0.18384431888586628</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA3">
+        <v>7.5417299416751529E-2</v>
+      </c>
+      <c r="AB3">
+        <v>0.17040300551471324</v>
+      </c>
+      <c r="AC3">
+        <v>0.30892317951245762</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>6.018467485076421</v>
       </c>
@@ -718,8 +745,17 @@
       <c r="Z4">
         <v>-3.8034768289925983E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA4">
+        <v>-2.2205886473895663E-2</v>
+      </c>
+      <c r="AB4">
+        <v>-5.1680790818715176E-2</v>
+      </c>
+      <c r="AC4">
+        <v>-6.2546097767217909E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5.247483015604316</v>
       </c>
@@ -798,8 +834,17 @@
       <c r="Z5">
         <v>-0.1383377138231599</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA5">
+        <v>-0.25019975922847265</v>
+      </c>
+      <c r="AB5">
+        <v>4.0855958763070993E-2</v>
+      </c>
+      <c r="AC5">
+        <v>3.4218350481499592E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4.7035328146850155</v>
       </c>
@@ -878,8 +923,17 @@
       <c r="Z6">
         <v>-9.4804460085001763E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA6">
+        <v>-1.1372256996764651E-2</v>
+      </c>
+      <c r="AB6">
+        <v>-0.41143189164290372</v>
+      </c>
+      <c r="AC6">
+        <v>-6.5635529133414749E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5.1450651475915423</v>
       </c>
@@ -958,8 +1012,17 @@
       <c r="Z7">
         <v>-0.19440434569067389</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA7">
+        <v>-0.13023498616240939</v>
+      </c>
+      <c r="AB7">
+        <v>-3.6343840849854814E-2</v>
+      </c>
+      <c r="AC7">
+        <v>-5.0796808854083025E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6.8699277510934751</v>
       </c>
@@ -1038,8 +1101,17 @@
       <c r="Z8">
         <v>-0.12597260064432517</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA8">
+        <v>-2.9090517165957584E-2</v>
+      </c>
+      <c r="AB8">
+        <v>-4.7339734371255743E-2</v>
+      </c>
+      <c r="AC8">
+        <v>0.21017534382972652</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6.0836476700778368</v>
       </c>
@@ -1118,8 +1190,17 @@
       <c r="Z9">
         <v>0.10910543613307265</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA9">
+        <v>-8.242578741522108E-3</v>
+      </c>
+      <c r="AB9">
+        <v>-4.2357872696248543E-2</v>
+      </c>
+      <c r="AC9">
+        <v>-5.6234225023866796E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5.3495359407153327</v>
       </c>
@@ -1198,8 +1279,17 @@
       <c r="Z10">
         <v>-0.35266942447163929</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA10">
+        <v>-0.37901895197426644</v>
+      </c>
+      <c r="AB10">
+        <v>0.12777653403398226</v>
+      </c>
+      <c r="AC10">
+        <v>9.2428991362448337E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6.9138568977452675</v>
       </c>
@@ -1278,8 +1368,17 @@
       <c r="Z11">
         <v>-0.20499756404349445</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA11">
+        <v>-0.18634755567494407</v>
+      </c>
+      <c r="AB11">
+        <v>-7.4238866175429782E-2</v>
+      </c>
+      <c r="AC11">
+        <v>1.1768255493800721E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3.2573753497478979</v>
       </c>
@@ -1358,8 +1457,17 @@
       <c r="Z12">
         <v>-0.25853474038174468</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA12">
+        <v>1.8988317678626347E-2</v>
+      </c>
+      <c r="AB12">
+        <v>2.2504715882848456E-2</v>
+      </c>
+      <c r="AC12">
+        <v>0.11587591876671857</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3.0065983171275397</v>
       </c>
@@ -1438,8 +1546,17 @@
       <c r="Z13">
         <v>0.14670505168581341</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA13">
+        <v>8.937822823207893E-2</v>
+      </c>
+      <c r="AB13">
+        <v>6.9181167246608902E-2</v>
+      </c>
+      <c r="AC13">
+        <v>-1.8223803011231755E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0.71754115055214318</v>
       </c>
@@ -1518,8 +1635,17 @@
       <c r="Z14">
         <v>7.0805972080918461E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA14">
+        <v>-4.548245312218477E-3</v>
+      </c>
+      <c r="AB14">
+        <v>0.11415634840701076</v>
+      </c>
+      <c r="AC14">
+        <v>0.15501713461584285</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2.1044405408727829</v>
       </c>
@@ -1598,8 +1724,17 @@
       <c r="Z15">
         <v>-0.28489160874806019</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA15">
+        <v>-6.6687719382675778E-3</v>
+      </c>
+      <c r="AB15">
+        <v>-0.15979183571763367</v>
+      </c>
+      <c r="AC15">
+        <v>-0.1265817242727372</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>5.3375523744066609</v>
       </c>
@@ -1678,8 +1813,17 @@
       <c r="Z16">
         <v>0.5816440569062149</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA16">
+        <v>-0.20810000417605568</v>
+      </c>
+      <c r="AB16">
+        <v>-6.0537820518456041E-2</v>
+      </c>
+      <c r="AC16">
+        <v>1.7851991443201078E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>5.5456267991679491</v>
       </c>
@@ -1758,8 +1902,17 @@
       <c r="Z17">
         <v>-0.23591292241075359</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA17">
+        <v>-7.6448759602950722E-2</v>
+      </c>
+      <c r="AB17">
+        <v>0.1287247496088347</v>
+      </c>
+      <c r="AC17">
+        <v>0.11510236170737342</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>7.475586993741909</v>
       </c>
@@ -1838,8 +1991,17 @@
       <c r="Z18">
         <v>-2.9697104717018405E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA18">
+        <v>3.9947975517555852E-3</v>
+      </c>
+      <c r="AB18">
+        <v>-0.16025990690782646</v>
+      </c>
+      <c r="AC18">
+        <v>-0.15740166980842102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>6.9519917573460788</v>
       </c>
@@ -1918,8 +2080,17 @@
       <c r="Z19">
         <v>-0.26323697118414846</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA19">
+        <v>-0.20734409788929337</v>
+      </c>
+      <c r="AB19">
+        <v>-0.20927232129450846</v>
+      </c>
+      <c r="AC19">
+        <v>-0.12224919940132009</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>7.3347616640913058</v>
       </c>
@@ -1998,8 +2169,17 @@
       <c r="Z20">
         <v>-0.25166240136946294</v>
       </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA20">
+        <v>-0.19226687514175486</v>
+      </c>
+      <c r="AB20">
+        <v>4.9716433892403105E-3</v>
+      </c>
+      <c r="AC20">
+        <v>2.4055797653996059E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>7.2161630144595641</v>
       </c>
@@ -2078,8 +2258,17 @@
       <c r="Z21">
         <v>-4.9216618366928588E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA21">
+        <v>1.8412404971732799E-2</v>
+      </c>
+      <c r="AB21">
+        <v>-5.7701836679014934E-2</v>
+      </c>
+      <c r="AC21">
+        <v>0.12921452255985749</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>7.3132826744032835</v>
       </c>
@@ -2158,8 +2347,17 @@
       <c r="Z22">
         <v>4.318667443041628E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA22">
+        <v>4.9550828637134024E-2</v>
+      </c>
+      <c r="AB22">
+        <v>-5.601962206283622E-2</v>
+      </c>
+      <c r="AC22">
+        <v>-3.2226963041208999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>7.874401341794858</v>
       </c>
@@ -2238,8 +2436,17 @@
       <c r="Z23">
         <v>-0.37410367762590052</v>
       </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA23">
+        <v>-4.3987104121763716E-2</v>
+      </c>
+      <c r="AB23">
+        <v>0.28125065045491088</v>
+      </c>
+      <c r="AC23">
+        <v>0.22684940643489207</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>8.1786843194554368</v>
       </c>
@@ -2318,8 +2525,17 @@
       <c r="Z24">
         <v>0.21048124882898581</v>
       </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA24">
+        <v>6.5234460548133505E-2</v>
+      </c>
+      <c r="AB24">
+        <v>-6.5810490274726116E-2</v>
+      </c>
+      <c r="AC24">
+        <v>2.0902395701531146E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>8.0728070541582877</v>
       </c>
@@ -2398,8 +2614,17 @@
       <c r="Z25">
         <v>0.28553897685940388</v>
       </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA25">
+        <v>-0.28267490780420285</v>
+      </c>
+      <c r="AB25">
+        <v>-0.112195721688561</v>
+      </c>
+      <c r="AC25">
+        <v>9.6794238903818997E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>7.5533476488074163</v>
       </c>
@@ -2478,8 +2703,17 @@
       <c r="Z26">
         <v>-0.24366405864284935</v>
       </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA26">
+        <v>0.12324986684940045</v>
+      </c>
+      <c r="AB26">
+        <v>-6.5753894993967596E-2</v>
+      </c>
+      <c r="AC26">
+        <v>-0.19636523680680376</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>8.5279406555946231</v>
       </c>
@@ -2558,8 +2792,17 @@
       <c r="Z27">
         <v>-6.4774850569603391E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA27">
+        <v>-4.0059169391712106E-2</v>
+      </c>
+      <c r="AB27">
+        <v>0.13372954656588279</v>
+      </c>
+      <c r="AC27">
+        <v>0.22015075708826151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>8.0801390144090952</v>
       </c>
@@ -2638,8 +2881,17 @@
       <c r="Z28">
         <v>-0.28460012741263102</v>
       </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA28">
+        <v>-9.6823127569391584E-2</v>
+      </c>
+      <c r="AB28">
+        <v>6.0062215334408062E-3</v>
+      </c>
+      <c r="AC28">
+        <v>0.1747928078804048</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>7.3681698011478041</v>
       </c>
@@ -2718,8 +2970,17 @@
       <c r="Z29">
         <v>-0.11363823261180757</v>
       </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA29">
+        <v>-0.10801308258337701</v>
+      </c>
+      <c r="AB29">
+        <v>3.1411253833763274E-2</v>
+      </c>
+      <c r="AC29">
+        <v>-8.4646409915375184E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>7.8852104089547019</v>
       </c>
@@ -2798,8 +3059,17 @@
       <c r="Z30">
         <v>-0.18173783027095514</v>
       </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA30">
+        <v>0.14836535089242708</v>
+      </c>
+      <c r="AB30">
+        <v>-3.1594375313917192E-2</v>
+      </c>
+      <c r="AC30">
+        <v>-4.0697050425791519E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>6.6241355388540564</v>
       </c>
@@ -2878,8 +3148,17 @@
       <c r="Z31">
         <v>-0.37220530958622233</v>
       </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA31">
+        <v>-0.33131685862835442</v>
+      </c>
+      <c r="AB31">
+        <v>-0.12583358403545869</v>
+      </c>
+      <c r="AC31">
+        <v>0.2599527778664002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>7.7998502329143289</v>
       </c>
@@ -2958,8 +3237,17 @@
       <c r="Z32">
         <v>-2.6951662427618052E-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA32">
+        <v>-0.12867302695814872</v>
+      </c>
+      <c r="AB32">
+        <v>-0.37326961923852664</v>
+      </c>
+      <c r="AC32">
+        <v>-0.23281429508865539</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>7.9648884925614016</v>
       </c>
@@ -3038,8 +3326,17 @@
       <c r="Z33">
         <v>-4.8282080476684038E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA33">
+        <v>0.11256955472456265</v>
+      </c>
+      <c r="AB33">
+        <v>-4.3909702372232677E-2</v>
+      </c>
+      <c r="AC33">
+        <v>-0.15015392841805733</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>7.9632941851649672</v>
       </c>
@@ -3118,8 +3415,17 @@
       <c r="Z34">
         <v>-0.23547366631175148</v>
       </c>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA34">
+        <v>-0.14328319549039598</v>
+      </c>
+      <c r="AB34">
+        <v>-8.1086350253592232E-2</v>
+      </c>
+      <c r="AC34">
+        <v>-0.17612237908437542</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>8.0433116124888375</v>
       </c>
@@ -3198,8 +3504,17 @@
       <c r="Z35">
         <v>4.5787268754595677E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA35">
+        <v>3.6267027125775148E-2</v>
+      </c>
+      <c r="AB35">
+        <v>-2.8004578454706056E-2</v>
+      </c>
+      <c r="AC35">
+        <v>-5.4540674421668968E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>6.7975664980586732</v>
       </c>
@@ -3278,8 +3593,17 @@
       <c r="Z36">
         <v>0.31392403173080896</v>
       </c>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA36">
+        <v>0.17329687704886237</v>
+      </c>
+      <c r="AB36">
+        <v>0.29536650269902187</v>
+      </c>
+      <c r="AC36">
+        <v>7.8496451259609482E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>8.1335566593649418</v>
       </c>
@@ -3358,8 +3682,17 @@
       <c r="Z37">
         <v>0.23052404908831126</v>
       </c>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA37">
+        <v>0.13673879218540055</v>
+      </c>
+      <c r="AB37">
+        <v>-6.9794430768584007E-2</v>
+      </c>
+      <c r="AC37">
+        <v>-8.5505146080733591E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>8.1335567793154269</v>
       </c>
@@ -3438,8 +3771,17 @@
       <c r="Z38">
         <v>0.22828456997256719</v>
       </c>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA38">
+        <v>0.13429760709704699</v>
+      </c>
+      <c r="AB38">
+        <v>-7.0871092013569212E-2</v>
+      </c>
+      <c r="AC38">
+        <v>-8.6479004567750581E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>6.6018539133853453</v>
       </c>
@@ -3518,8 +3860,17 @@
       <c r="Z39">
         <v>-3.6449778256065976E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA39">
+        <v>0.12149267987725591</v>
+      </c>
+      <c r="AB39">
+        <v>-1.3081166890383508E-2</v>
+      </c>
+      <c r="AC39">
+        <v>-0.17695252728179461</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>6.9714441301523822</v>
       </c>
@@ -3598,8 +3949,17 @@
       <c r="Z40">
         <v>0.23682657521872957</v>
       </c>
-    </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA40">
+        <v>0.15287929312878715</v>
+      </c>
+      <c r="AB40">
+        <v>-4.5467521326853652E-2</v>
+      </c>
+      <c r="AC40">
+        <v>-6.7954629321162627E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>6.8537300387176154</v>
       </c>
@@ -3678,8 +4038,17 @@
       <c r="Z41">
         <v>0.30412685180568405</v>
       </c>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA41">
+        <v>0.2318660056192326</v>
+      </c>
+      <c r="AB41">
+        <v>-7.6032113703111581E-2</v>
+      </c>
+      <c r="AC41">
+        <v>-0.19241129960518644</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>8.4033294011678379</v>
       </c>
@@ -3758,8 +4127,17 @@
       <c r="Z42">
         <v>0.22379042992251055</v>
       </c>
-    </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA42">
+        <v>7.2299848711515458E-2</v>
+      </c>
+      <c r="AB42">
+        <v>1.8068404053448176E-2</v>
+      </c>
+      <c r="AC42">
+        <v>2.8931457106447265E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>7.2769286249046017</v>
       </c>
@@ -3838,8 +4216,17 @@
       <c r="Z43">
         <v>-0.13656052783617462</v>
       </c>
-    </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA43">
+        <v>-8.284899328929915E-2</v>
+      </c>
+      <c r="AB43">
+        <v>-0.29902323221786792</v>
+      </c>
+      <c r="AC43">
+        <v>0.20675338898868906</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>7.7116543491460074</v>
       </c>
@@ -3918,8 +4305,17 @@
       <c r="Z44">
         <v>-3.9176314488783635E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA44">
+        <v>0.13703736200315089</v>
+      </c>
+      <c r="AB44">
+        <v>7.3082937441717233E-2</v>
+      </c>
+      <c r="AC44">
+        <v>-0.22312516518041917</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>7.6141438061978954</v>
       </c>
@@ -3998,8 +4394,17 @@
       <c r="Z45">
         <v>7.0681327998524016E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA45">
+        <v>6.6162117458071198E-2</v>
+      </c>
+      <c r="AB45">
+        <v>-0.13280292211909384</v>
+      </c>
+      <c r="AC45">
+        <v>1.1373994401400316E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>3.4911349770034432</v>
       </c>
@@ -4078,8 +4483,17 @@
       <c r="Z46">
         <v>-0.1637655249972079</v>
       </c>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA46">
+        <v>4.4347348255364016E-2</v>
+      </c>
+      <c r="AB46">
+        <v>0.11110090807028118</v>
+      </c>
+      <c r="AC46">
+        <v>2.9054634332121802E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>4.465649716499799</v>
       </c>
@@ -4158,8 +4572,17 @@
       <c r="Z47">
         <v>0.14779638262801836</v>
       </c>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA47">
+        <v>-0.12649336060721542</v>
+      </c>
+      <c r="AB47">
+        <v>-0.14501220142044091</v>
+      </c>
+      <c r="AC47">
+        <v>-0.1582854888907673</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>6.1649430018671181</v>
       </c>
@@ -4238,8 +4661,17 @@
       <c r="Z48">
         <v>-5.9915851412299957E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA48">
+        <v>7.0291106251508584E-2</v>
+      </c>
+      <c r="AB48">
+        <v>-2.3474724176583313E-2</v>
+      </c>
+      <c r="AC48">
+        <v>-8.6677990160058824E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>5.8994484812142138</v>
       </c>
@@ -4318,8 +4750,17 @@
       <c r="Z49">
         <v>-2.6806209388334432E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA49">
+        <v>-3.8554152754966604E-2</v>
+      </c>
+      <c r="AB49">
+        <v>0.11745729358801205</v>
+      </c>
+      <c r="AC49">
+        <v>0.1872282774704371</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>4.9659151281152809</v>
       </c>
@@ -4398,8 +4839,17 @@
       <c r="Z50">
         <v>-0.12081293985455324</v>
       </c>
-    </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA50">
+        <v>-6.2482577321827083E-2</v>
+      </c>
+      <c r="AB50">
+        <v>0.11477324834702628</v>
+      </c>
+      <c r="AC50">
+        <v>4.6462543374315372E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>4.8975373535075626</v>
       </c>
@@ -4478,8 +4928,17 @@
       <c r="Z51">
         <v>-0.31170528124903923</v>
       </c>
-    </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA51">
+        <v>0.11584985025852265</v>
+      </c>
+      <c r="AB51">
+        <v>-0.12148490345367838</v>
+      </c>
+      <c r="AC51">
+        <v>1.6389075889222691E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>4.2268337208362574</v>
       </c>
@@ -4558,8 +5017,17 @@
       <c r="Z52">
         <v>-0.22979763373837458</v>
       </c>
-    </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA52">
+        <v>-8.6090615139907782E-3</v>
+      </c>
+      <c r="AB52">
+        <v>0.16807769106142775</v>
+      </c>
+      <c r="AC52">
+        <v>2.7278257821262256E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>4.567371309297636</v>
       </c>
@@ -4638,8 +5106,17 @@
       <c r="Z53">
         <v>-4.2785422880298372E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA53">
+        <v>-0.30453908539636265</v>
+      </c>
+      <c r="AB53">
+        <v>-4.7085705434914873E-2</v>
+      </c>
+      <c r="AC53">
+        <v>-5.809819459991572E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>5.3283275822390621</v>
       </c>
@@ -4718,8 +5195,17 @@
       <c r="Z54">
         <v>-0.1149118251314635</v>
       </c>
-    </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA54">
+        <v>3.4684286855206845E-2</v>
+      </c>
+      <c r="AB54">
+        <v>-7.9210570584683268E-2</v>
+      </c>
+      <c r="AC54">
+        <v>-0.23296965266206676</v>
+      </c>
+    </row>
+    <row r="55" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>5.7624104505873097</v>
       </c>
@@ -4798,8 +5284,17 @@
       <c r="Z55">
         <v>1.2864119257483847E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA55">
+        <v>8.7197250430974399E-3</v>
+      </c>
+      <c r="AB55">
+        <v>-0.14551543960701288</v>
+      </c>
+      <c r="AC55">
+        <v>-8.3737818437239361E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>5.312246103956145</v>
       </c>
@@ -4878,8 +5373,17 @@
       <c r="Z56">
         <v>-8.7194863990830481E-3</v>
       </c>
-    </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA56">
+        <v>3.3450202113131031E-2</v>
+      </c>
+      <c r="AB56">
+        <v>7.6870179283379636E-2</v>
+      </c>
+      <c r="AC56">
+        <v>0.19069271229977641</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>6.7291600463018018</v>
       </c>
@@ -4958,8 +5462,17 @@
       <c r="Z57">
         <v>0.22118817486492393</v>
       </c>
-    </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA57">
+        <v>-0.16553125707480806</v>
+      </c>
+      <c r="AB57">
+        <v>3.0148286680561475E-2</v>
+      </c>
+      <c r="AC57">
+        <v>-3.0954397344027221E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>7.0091831903401989</v>
       </c>
@@ -5038,8 +5551,17 @@
       <c r="Z58">
         <v>6.9602256941514534E-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA58">
+        <v>-7.9169093375056673E-4</v>
+      </c>
+      <c r="AB58">
+        <v>0.11047499912976394</v>
+      </c>
+      <c r="AC58">
+        <v>8.2870553386366202E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>6.8501430683817093</v>
       </c>
@@ -5118,8 +5640,17 @@
       <c r="Z59">
         <v>-0.20959228183127024</v>
       </c>
-    </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA59">
+        <v>-5.4398226950655715E-2</v>
+      </c>
+      <c r="AB59">
+        <v>4.1997178738358919E-2</v>
+      </c>
+      <c r="AC59">
+        <v>-6.2383785168040849E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>6.5459979302005973</v>
       </c>
@@ -5198,8 +5729,17 @@
       <c r="Z60">
         <v>-0.23218597058524199</v>
       </c>
-    </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA60">
+        <v>-0.34693072800184055</v>
+      </c>
+      <c r="AB60">
+        <v>-0.16862888887123795</v>
+      </c>
+      <c r="AC60">
+        <v>0.23059550923413422</v>
+      </c>
+    </row>
+    <row r="61" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>5.5564798991598146</v>
       </c>
@@ -5278,8 +5818,17 @@
       <c r="Z61">
         <v>0.10123200678428183</v>
       </c>
-    </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA61">
+        <v>-2.9533499210263745E-2</v>
+      </c>
+      <c r="AB61">
+        <v>-1.2514871397557533E-3</v>
+      </c>
+      <c r="AC61">
+        <v>0.1406597390316251</v>
+      </c>
+    </row>
+    <row r="62" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>6.918086387610189</v>
       </c>
@@ -5358,8 +5907,17 @@
       <c r="Z62">
         <v>0.26360634609942618</v>
       </c>
-    </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA62">
+        <v>1.6821656214148835E-2</v>
+      </c>
+      <c r="AB62">
+        <v>-5.9138380692086198E-2</v>
+      </c>
+      <c r="AC62">
+        <v>4.1078588523761103E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>4.4371885282251684</v>
       </c>
@@ -5438,8 +5996,17 @@
       <c r="Z63">
         <v>-8.6037979479655496E-2</v>
       </c>
-    </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA63">
+        <v>-0.11853645506503852</v>
+      </c>
+      <c r="AB63">
+        <v>-1.2496418670117771E-2</v>
+      </c>
+      <c r="AC63">
+        <v>-3.3260532217023291E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>6.179765030800314</v>
       </c>
@@ -5518,8 +6085,17 @@
       <c r="Z64">
         <v>0.10111354829610841</v>
       </c>
-    </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA64">
+        <v>3.5107048422241549E-2</v>
+      </c>
+      <c r="AB64">
+        <v>-0.21093133344993326</v>
+      </c>
+      <c r="AC64">
+        <v>-0.29017352003321667</v>
+      </c>
+    </row>
+    <row r="65" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>7.8125104677148229</v>
       </c>
@@ -5598,8 +6174,17 @@
       <c r="Z65">
         <v>-1.2567104319042206E-3</v>
       </c>
-    </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA65">
+        <v>0.1117323431038294</v>
+      </c>
+      <c r="AB65">
+        <v>6.0186648408203092E-2</v>
+      </c>
+      <c r="AC65">
+        <v>-9.3951408506212045E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>6.4900679845879043</v>
       </c>
@@ -5678,8 +6263,17 @@
       <c r="Z66">
         <v>-0.13184240315177304</v>
       </c>
-    </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA66">
+        <v>4.4029804855427714E-2</v>
+      </c>
+      <c r="AB66">
+        <v>-0.19038107516532188</v>
+      </c>
+      <c r="AC66">
+        <v>7.0033915632672326E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>1.5396152819952365</v>
       </c>
@@ -5758,8 +6352,17 @@
       <c r="Z67">
         <v>8.1776577371919668E-3</v>
       </c>
-    </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA67">
+        <v>0.41832271250870984</v>
+      </c>
+      <c r="AB67">
+        <v>5.9161493030081627E-2</v>
+      </c>
+      <c r="AC67">
+        <v>0.21388733663059978</v>
+      </c>
+    </row>
+    <row r="68" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>6.8024013863956236</v>
       </c>
@@ -5838,8 +6441,17 @@
       <c r="Z68">
         <v>-0.24381817455674379</v>
       </c>
-    </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA68">
+        <v>-0.27193247284989319</v>
+      </c>
+      <c r="AB68">
+        <v>3.360365169319917E-2</v>
+      </c>
+      <c r="AC68">
+        <v>0.11575210054273008</v>
+      </c>
+    </row>
+    <row r="69" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>7.1846730346256731</v>
       </c>
@@ -5918,8 +6530,17 @@
       <c r="Z69">
         <v>-8.5223964375795505E-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA69">
+        <v>-0.23587339654420289</v>
+      </c>
+      <c r="AB69">
+        <v>-0.15061453245481685</v>
+      </c>
+      <c r="AC69">
+        <v>2.9379520345162311E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>5.8845270903957561</v>
       </c>
@@ -5998,8 +6619,17 @@
       <c r="Z70">
         <v>-9.3845763589849598E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA70">
+        <v>5.408379492906689E-2</v>
+      </c>
+      <c r="AB70">
+        <v>-8.070400289610935E-2</v>
+      </c>
+      <c r="AC70">
+        <v>9.1422409231409749E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>6.0174244582082794</v>
       </c>
@@ -6078,8 +6708,17 @@
       <c r="Z71">
         <v>-0.11638493193217016</v>
       </c>
-    </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA71">
+        <v>6.3854665419325093E-2</v>
+      </c>
+      <c r="AB71">
+        <v>9.2419304535780428E-2</v>
+      </c>
+      <c r="AC71">
+        <v>1.5914079803939486E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>6.2098627410367166</v>
       </c>
@@ -6158,8 +6797,17 @@
       <c r="Z72">
         <v>-0.11558992644002579</v>
       </c>
-    </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA72">
+        <v>-0.13947571891693436</v>
+      </c>
+      <c r="AB72">
+        <v>-8.5730725892775861E-2</v>
+      </c>
+      <c r="AC72">
+        <v>-0.17999386100815534</v>
+      </c>
+    </row>
+    <row r="73" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>4.3988107439550923</v>
       </c>
@@ -6238,8 +6886,17 @@
       <c r="Z73">
         <v>-2.8745982832048992E-2</v>
       </c>
-    </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA73">
+        <v>0.240767630125584</v>
+      </c>
+      <c r="AB73">
+        <v>-0.14583380943816751</v>
+      </c>
+      <c r="AC73">
+        <v>0.12307547319678495</v>
+      </c>
+    </row>
+    <row r="74" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>6.6752958086959211</v>
       </c>
@@ -6318,8 +6975,17 @@
       <c r="Z74">
         <v>0.39955281119337455</v>
       </c>
-    </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA74">
+        <v>-0.41283988644073027</v>
+      </c>
+      <c r="AB74">
+        <v>0.4501873595745613</v>
+      </c>
+      <c r="AC74">
+        <v>-0.25926759268906285</v>
+      </c>
+    </row>
+    <row r="75" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>6.1745448820278863</v>
       </c>
@@ -6398,46 +7064,55 @@
       <c r="Z75">
         <v>-0.27965506242142729</v>
       </c>
-    </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA75">
+        <v>0.26455933212002658</v>
+      </c>
+      <c r="AB75">
+        <v>-8.2629033916698069E-2</v>
+      </c>
+      <c r="AC75">
+        <v>7.0061598007029505E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>2.9358196690473326</v>
+        <v>6.2098627410367166</v>
       </c>
       <c r="B76">
-        <v>2.7249673185869683</v>
+        <v>-0.21063689765620119</v>
       </c>
       <c r="C76">
-        <v>-2.2695019536399363</v>
+        <v>-1.370192447328364</v>
       </c>
       <c r="D76">
-        <v>-2.0003256163147172</v>
+        <v>-0.84887844051040218</v>
       </c>
       <c r="E76">
-        <v>-0.53808010586409316</v>
+        <v>-4.8931700186480985E-2</v>
       </c>
       <c r="F76">
-        <v>-0.24785610663116933</v>
+        <v>0.57186918221178451</v>
       </c>
       <c r="G76">
-        <v>-3.7791560230077313E-2</v>
+        <v>-0.13774776864740526</v>
       </c>
       <c r="H76">
-        <v>-0.56832159942335536</v>
+        <v>-0.45637385917520484</v>
       </c>
       <c r="I76">
-        <v>-0.81309168560139522</v>
+        <v>-0.32336006554088187</v>
       </c>
       <c r="J76">
-        <v>-0.69463040716092228</v>
+        <v>-0.4194173754525044</v>
       </c>
       <c r="K76">
-        <v>-0.55054912415288226</v>
+        <v>-0.22584345975083714</v>
       </c>
       <c r="L76">
-        <v>-0.39805093067874447</v>
+        <v>0.26809883573587651</v>
       </c>
       <c r="M76">
-        <v>1.3186665216587095E-3</v>
+        <v>-0.32959840886643732</v>
       </c>
       <c r="N76">
         <v>0.14926109581446481</v>
@@ -6479,45 +7154,45 @@
         <v>0.1300593934084609</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>5.8819256675879554</v>
+        <v>4.3988107439550923</v>
       </c>
       <c r="B77">
-        <v>-0.99557297978974379</v>
+        <v>-3.9224824693888038</v>
       </c>
       <c r="C77">
-        <v>-2.8593622489065864</v>
+        <v>-3.2512351757241751</v>
       </c>
       <c r="D77">
-        <v>-1.7814787345951204</v>
+        <v>2.1284776558237364</v>
       </c>
       <c r="E77">
-        <v>-0.15668587787902064</v>
+        <v>-0.57342544969585429</v>
       </c>
       <c r="F77">
-        <v>0.52806708841063987</v>
+        <v>5.8583486340814526E-2</v>
       </c>
       <c r="G77">
-        <v>0.74468230047669404</v>
+        <v>0.29539355656182564</v>
       </c>
       <c r="H77">
-        <v>0.40238815986433085</v>
+        <v>8.2154698670005119E-2</v>
       </c>
       <c r="I77">
-        <v>3.2048610136147578E-2</v>
+        <v>-0.83328030147300836</v>
       </c>
       <c r="J77">
-        <v>-0.13768575255148749</v>
+        <v>0.33873931586527029</v>
       </c>
       <c r="K77">
-        <v>-0.61149198407657601</v>
+        <v>0.36977583099050193</v>
       </c>
       <c r="L77">
-        <v>-0.38202325172840967</v>
+        <v>-0.31673523074388277</v>
       </c>
       <c r="M77">
-        <v>0.13718563573437342</v>
+        <v>3.7439664969409229E-3</v>
       </c>
       <c r="N77">
         <v>0.17266829637743461</v>
@@ -6559,45 +7234,45 @@
         <v>-4.5340511212256787E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>4.7429380835678172</v>
+        <v>6.6752958086959211</v>
       </c>
       <c r="B78">
-        <v>-1.4809513510871186</v>
+        <v>-5.6811879971357611</v>
       </c>
       <c r="C78">
-        <v>-2.5135324841624067</v>
+        <v>-1.7878377798288585</v>
       </c>
       <c r="D78">
-        <v>0.66883450600431804</v>
+        <v>1.7601031196399719</v>
       </c>
       <c r="E78">
-        <v>-2.3910518728873527</v>
+        <v>-0.74109973503995008</v>
       </c>
       <c r="F78">
-        <v>1.3918719702356044</v>
+        <v>2.3169995808848216E-2</v>
       </c>
       <c r="G78">
-        <v>-0.3022660752861161</v>
+        <v>-9.4804575140565506E-2</v>
       </c>
       <c r="H78">
-        <v>-0.32386238377178522</v>
+        <v>0.53662763391245261</v>
       </c>
       <c r="I78">
-        <v>0.20786102105536688</v>
+        <v>-1.004199503615181</v>
       </c>
       <c r="J78">
-        <v>4.253343354906005E-2</v>
+        <v>0.98309982010817365</v>
       </c>
       <c r="K78">
-        <v>-0.28893032713396077</v>
+        <v>5.486273678109675E-3</v>
       </c>
       <c r="L78">
-        <v>0.51639587922948027</v>
+        <v>-0.54629282925006473</v>
       </c>
       <c r="M78">
-        <v>-9.6932376841417534E-2</v>
+        <v>-0.42885775757814842</v>
       </c>
       <c r="N78">
         <v>-0.20365101888706491</v>
@@ -6639,45 +7314,45 @@
         <v>1.1154292143552137E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>4.424582198244063</v>
+        <v>6.1745448820278863</v>
       </c>
       <c r="B79">
-        <v>-2.8669506080834242</v>
+        <v>-6.2068913846709206</v>
       </c>
       <c r="C79">
-        <v>0.68070102373195085</v>
+        <v>-3.9022999946664849</v>
       </c>
       <c r="D79">
-        <v>-1.0487966339053678</v>
+        <v>2.6312168499107229</v>
       </c>
       <c r="E79">
-        <v>0.7758350013682288</v>
+        <v>-1.7278193673320037</v>
       </c>
       <c r="F79">
-        <v>-0.14897455941101445</v>
+        <v>-5.1155515543705239E-2</v>
       </c>
       <c r="G79">
-        <v>0.36368461062830298</v>
+        <v>-7.6009484362449919E-2</v>
       </c>
       <c r="H79">
-        <v>0.25085598987556668</v>
+        <v>-0.18168243234455178</v>
       </c>
       <c r="I79">
-        <v>0.29059768038871975</v>
+        <v>-0.69585850341701772</v>
       </c>
       <c r="J79">
-        <v>0.72867212274274251</v>
+        <v>0.12782670448526534</v>
       </c>
       <c r="K79">
-        <v>0.40023444098039501</v>
+        <v>0.43659976979246923</v>
       </c>
       <c r="L79">
-        <v>0.29313138647937409</v>
+        <v>0.80763402934231265</v>
       </c>
       <c r="M79">
-        <v>0.1953516919519761</v>
+        <v>-1.0430182097657761</v>
       </c>
       <c r="N79">
         <v>-1.4194466354636618E-2</v>
@@ -6719,45 +7394,45 @@
         <v>3.7347205667917292E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>5.670102301558912</v>
+        <v>2.7156900536869877</v>
       </c>
       <c r="B80">
-        <v>-0.58547045742392512</v>
+        <v>1.7529324208448611</v>
       </c>
       <c r="C80">
-        <v>-1.5310314435237793</v>
+        <v>-1.8665463334255123</v>
       </c>
       <c r="D80">
-        <v>-1.1486715412029158</v>
+        <v>-0.53171216903513796</v>
       </c>
       <c r="E80">
-        <v>-2.3466711332336203</v>
+        <v>5.9988193998202585E-2</v>
       </c>
       <c r="F80">
-        <v>-1.6784237652031615</v>
+        <v>0.91586102162647298</v>
       </c>
       <c r="G80">
-        <v>-1.4857074100820673</v>
+        <v>0.4450457266556952</v>
       </c>
       <c r="H80">
-        <v>-0.73556613559075112</v>
+        <v>-0.24521364271057428</v>
       </c>
       <c r="I80">
-        <v>6.3160645467374057E-2</v>
+        <v>0.92027882711550535</v>
       </c>
       <c r="J80">
-        <v>-1.7609099981775272E-2</v>
+        <v>0.30281541866059608</v>
       </c>
       <c r="K80">
-        <v>0.79183610993840725</v>
+        <v>0.23933590338446598</v>
       </c>
       <c r="L80">
-        <v>0.44677986600472275</v>
+        <v>0.31569152863045924</v>
       </c>
       <c r="M80">
-        <v>0.27739670508292036</v>
+        <v>-0.26669156530070481</v>
       </c>
       <c r="N80">
         <v>-0.18224965850908897</v>
@@ -6801,43 +7476,43 @@
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>6.7193733668586066</v>
+        <v>4.3988107439550923</v>
       </c>
       <c r="B81">
-        <v>3.5301805414258167</v>
+        <v>-3.9224824693888038</v>
       </c>
       <c r="C81">
-        <v>-0.38726681023914356</v>
+        <v>-3.2512351757241751</v>
       </c>
       <c r="D81">
-        <v>-0.51398021959479956</v>
+        <v>2.1284776558237364</v>
       </c>
       <c r="E81">
-        <v>-1.5794457472412091</v>
+        <v>-0.57342544969585429</v>
       </c>
       <c r="F81">
-        <v>-1.3990086006209497</v>
+        <v>5.8583486340814526E-2</v>
       </c>
       <c r="G81">
-        <v>-0.44901188617589616</v>
+        <v>0.29539355656182564</v>
       </c>
       <c r="H81">
-        <v>-0.22392129451455192</v>
+        <v>8.2154698670005119E-2</v>
       </c>
       <c r="I81">
-        <v>0.2732259237301532</v>
+        <v>-0.83328030147300836</v>
       </c>
       <c r="J81">
-        <v>0.88228515229958115</v>
+        <v>0.33873931586527029</v>
       </c>
       <c r="K81">
-        <v>-9.6859393963611401E-2</v>
+        <v>0.36977583099050193</v>
       </c>
       <c r="L81">
-        <v>0.2613606950208629</v>
+        <v>-0.31673523074388277</v>
       </c>
       <c r="M81">
-        <v>-0.17570861157819587</v>
+        <v>3.7439664969409229E-3</v>
       </c>
       <c r="N81">
         <v>0.36948530212218383</v>
@@ -6881,43 +7556,43 @@
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>5.3321000682762891</v>
+        <v>6.6752958086959211</v>
       </c>
       <c r="B82">
-        <v>1.7048277565540924</v>
+        <v>-5.6811879971357611</v>
       </c>
       <c r="C82">
-        <v>-1.6578250404282167</v>
+        <v>-1.7878377798288585</v>
       </c>
       <c r="D82">
-        <v>-2.0616336761959557</v>
+        <v>1.7601031196399719</v>
       </c>
       <c r="E82">
-        <v>-1.4673173831495478</v>
+        <v>-0.74109973503995008</v>
       </c>
       <c r="F82">
-        <v>-2.4806188967972607</v>
+        <v>2.3169995808848216E-2</v>
       </c>
       <c r="G82">
-        <v>-0.97010963947730333</v>
+        <v>-9.4804575140565506E-2</v>
       </c>
       <c r="H82">
-        <v>-1.1074275882212536</v>
+        <v>0.53662763391245261</v>
       </c>
       <c r="I82">
-        <v>-0.17272049051057434</v>
+        <v>-1.004199503615181</v>
       </c>
       <c r="J82">
-        <v>0.43204561196586705</v>
+        <v>0.98309982010817365</v>
       </c>
       <c r="K82">
-        <v>0.38932566504079291</v>
+        <v>5.486273678109675E-3</v>
       </c>
       <c r="L82">
-        <v>0.27379932274449453</v>
+        <v>-0.54629282925006473</v>
       </c>
       <c r="M82">
-        <v>-0.15417956008774739</v>
+        <v>-0.42885775757814842</v>
       </c>
       <c r="N82">
         <v>0.58877518063384859</v>
@@ -6961,43 +7636,43 @@
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>6.352698349231181</v>
+        <v>6.1745448820278863</v>
       </c>
       <c r="B83">
-        <v>-0.94613995334573564</v>
+        <v>-6.2068913846709206</v>
       </c>
       <c r="C83">
-        <v>0.64785656563357963</v>
+        <v>-3.9022999946664849</v>
       </c>
       <c r="D83">
-        <v>-1.1107118228194941</v>
+        <v>2.6312168499107229</v>
       </c>
       <c r="E83">
-        <v>-2.5727203548687347</v>
+        <v>-1.7278193673320037</v>
       </c>
       <c r="F83">
-        <v>-0.44074158910752192</v>
+        <v>-5.1155515543705239E-2</v>
       </c>
       <c r="G83">
-        <v>-1.6360082522141406</v>
+        <v>-7.6009484362449919E-2</v>
       </c>
       <c r="H83">
-        <v>-0.14346924873262665</v>
+        <v>-0.18168243234455178</v>
       </c>
       <c r="I83">
-        <v>-6.4078700915544393E-2</v>
+        <v>-0.69585850341701772</v>
       </c>
       <c r="J83">
-        <v>0.92914701456602933</v>
+        <v>0.12782670448526534</v>
       </c>
       <c r="K83">
-        <v>0.32640279375870435</v>
+        <v>0.43659976979246923</v>
       </c>
       <c r="L83">
-        <v>0.15177671194331055</v>
+        <v>0.80763402934231265</v>
       </c>
       <c r="M83">
-        <v>-0.2990486902432809</v>
+        <v>-1.0430182097657761</v>
       </c>
       <c r="N83">
         <v>0.19813675305578407</v>
@@ -7041,43 +7716,43 @@
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>6.1198782184005314</v>
+        <v>2.7156900536869877</v>
       </c>
       <c r="B84">
-        <v>6.1871550335328136</v>
+        <v>1.7529324208448611</v>
       </c>
       <c r="C84">
-        <v>0.17273103454249311</v>
+        <v>-1.8665463334255123</v>
       </c>
       <c r="D84">
-        <v>0.33076636650281199</v>
+        <v>-0.53171216903513796</v>
       </c>
       <c r="E84">
-        <v>0.77547792304916052</v>
+        <v>5.9988193998202585E-2</v>
       </c>
       <c r="F84">
-        <v>0.7870980516345637</v>
+        <v>0.91586102162647298</v>
       </c>
       <c r="G84">
-        <v>8.0847805479929369E-2</v>
+        <v>0.4450457266556952</v>
       </c>
       <c r="H84">
-        <v>-0.24073120689691999</v>
+        <v>-0.24521364271057428</v>
       </c>
       <c r="I84">
-        <v>-0.27445709914482364</v>
+        <v>0.92027882711550535</v>
       </c>
       <c r="J84">
-        <v>-0.16868342545933954</v>
+        <v>0.30281541866059608</v>
       </c>
       <c r="K84">
-        <v>-0.13462757074671097</v>
+        <v>0.23933590338446598</v>
       </c>
       <c r="L84">
-        <v>-4.4700726697447783E-2</v>
+        <v>0.31569152863045924</v>
       </c>
       <c r="M84">
-        <v>-8.4963665066341856E-2</v>
+        <v>-0.26669156530070481</v>
       </c>
       <c r="N84">
         <v>-3.5345751552870869E-2</v>
@@ -7121,43 +7796,43 @@
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>7.1150747018702987</v>
+        <v>5.2245018140118349</v>
       </c>
       <c r="B85">
-        <v>3.1835709067668048</v>
+        <v>1.3478538778114693</v>
       </c>
       <c r="C85">
-        <v>2.2312417067126273</v>
+        <v>0.38139434061318156</v>
       </c>
       <c r="D85">
-        <v>-0.20986329245191165</v>
+        <v>3.5156730478015259</v>
       </c>
       <c r="E85">
-        <v>-0.84012134380000048</v>
+        <v>0.46855541743494672</v>
       </c>
       <c r="F85">
-        <v>0.51560936672739899</v>
+        <v>0.57977206825760619</v>
       </c>
       <c r="G85">
-        <v>7.4735461102481054E-2</v>
+        <v>0.30648016076600687</v>
       </c>
       <c r="H85">
-        <v>0.56621382813003263</v>
+        <v>0.17128645452943492</v>
       </c>
       <c r="I85">
-        <v>-1.5023516841362998</v>
+        <v>-1.0645346889563587</v>
       </c>
       <c r="J85">
-        <v>0.24106176663247281</v>
+        <v>-0.30871754638322252</v>
       </c>
       <c r="K85">
-        <v>-1.5199643747652405</v>
+        <v>6.556885397645551E-2</v>
       </c>
       <c r="L85">
-        <v>0.60359048823317341</v>
+        <v>-0.27175801828161245</v>
       </c>
       <c r="M85">
-        <v>-0.25424746341715732</v>
+        <v>-0.23366108666756749</v>
       </c>
       <c r="N85">
         <v>0.21748581312343948</v>
@@ -7201,43 +7876,43 @@
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>4.7638344903689021</v>
+        <v>6.6752958086959211</v>
       </c>
       <c r="B86">
-        <v>5.7220205133896833</v>
+        <v>-5.6811879971357611</v>
       </c>
       <c r="C86">
-        <v>0.55742153779201808</v>
+        <v>-1.7878377798288585</v>
       </c>
       <c r="D86">
-        <v>-0.78978062039396624</v>
+        <v>1.7601031196399719</v>
       </c>
       <c r="E86">
-        <v>-0.49731244510656097</v>
+        <v>-0.74109973503995008</v>
       </c>
       <c r="F86">
-        <v>-7.3632387479966005E-2</v>
+        <v>2.3169995808848216E-2</v>
       </c>
       <c r="G86">
-        <v>-0.47289889706323618</v>
+        <v>-9.4804575140565506E-2</v>
       </c>
       <c r="H86">
-        <v>-0.91543192513014626</v>
+        <v>0.53662763391245261</v>
       </c>
       <c r="I86">
-        <v>-0.85341157609503238</v>
+        <v>-1.004199503615181</v>
       </c>
       <c r="J86">
-        <v>-0.98511559865611698</v>
+        <v>0.98309982010817365</v>
       </c>
       <c r="K86">
-        <v>-0.76418656271671948</v>
+        <v>5.486273678109675E-3</v>
       </c>
       <c r="L86">
-        <v>-0.61154064921598306</v>
+        <v>-0.54629282925006473</v>
       </c>
       <c r="M86">
-        <v>-0.51306210703490207</v>
+        <v>-0.42885775757814842</v>
       </c>
       <c r="N86">
         <v>-5.829810645199432E-4</v>
@@ -7281,43 +7956,43 @@
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>4.4778001098962905</v>
+        <v>6.1745448820278863</v>
       </c>
       <c r="B87">
-        <v>6.1553017627434379</v>
+        <v>-6.2068913846709206</v>
       </c>
       <c r="C87">
-        <v>0.92057585331663361</v>
+        <v>-3.9022999946664849</v>
       </c>
       <c r="D87">
-        <v>0.64424019611188565</v>
+        <v>2.6312168499107229</v>
       </c>
       <c r="E87">
-        <v>0.60999078529979334</v>
+        <v>-1.7278193673320037</v>
       </c>
       <c r="F87">
-        <v>-0.64259349161334534</v>
+        <v>-5.1155515543705239E-2</v>
       </c>
       <c r="G87">
-        <v>-0.82292582226548971</v>
+        <v>-7.6009484362449919E-2</v>
       </c>
       <c r="H87">
-        <v>-0.52166732307217434</v>
+        <v>-0.18168243234455178</v>
       </c>
       <c r="I87">
-        <v>-0.59660631001890974</v>
+        <v>-0.69585850341701772</v>
       </c>
       <c r="J87">
-        <v>-0.72507844161070767</v>
+        <v>0.12782670448526534</v>
       </c>
       <c r="K87">
-        <v>-0.48326741856895938</v>
+        <v>0.43659976979246923</v>
       </c>
       <c r="L87">
-        <v>-0.50486479595086964</v>
+        <v>0.80763402934231265</v>
       </c>
       <c r="M87">
-        <v>-0.16074996996290092</v>
+        <v>-1.0430182097657761</v>
       </c>
       <c r="N87">
         <v>0.21666049372455737</v>
@@ -7361,43 +8036,43 @@
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>3.7040405543667165</v>
+        <v>2.7156900536869877</v>
       </c>
       <c r="B88">
-        <v>4.0100992996833176</v>
+        <v>1.7529324208448611</v>
       </c>
       <c r="C88">
-        <v>0.17028342864328833</v>
+        <v>-1.8665463334255123</v>
       </c>
       <c r="D88">
-        <v>0.54439143192218531</v>
+        <v>-0.53171216903513796</v>
       </c>
       <c r="E88">
-        <v>-0.73581925806281856</v>
+        <v>5.9988193998202585E-2</v>
       </c>
       <c r="F88">
-        <v>-0.1103057464998964</v>
+        <v>0.91586102162647298</v>
       </c>
       <c r="G88">
-        <v>0.22016725288063699</v>
+        <v>0.4450457266556952</v>
       </c>
       <c r="H88">
-        <v>-1.2766581948845928</v>
+        <v>-0.24521364271057428</v>
       </c>
       <c r="I88">
-        <v>-0.67236834393587264</v>
+        <v>0.92027882711550535</v>
       </c>
       <c r="J88">
-        <v>2.7033037507317417E-2</v>
+        <v>0.30281541866059608</v>
       </c>
       <c r="K88">
-        <v>-0.89210279166783601</v>
+        <v>0.23933590338446598</v>
       </c>
       <c r="L88">
-        <v>-0.1156605140918298</v>
+        <v>0.31569152863045924</v>
       </c>
       <c r="M88">
-        <v>0.17675881676142366</v>
+        <v>-0.26669156530070481</v>
       </c>
       <c r="N88">
         <v>-0.65993150394586131</v>
@@ -7441,43 +8116,43 @@
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>2.2408153429736686</v>
+        <v>5.2245018140118349</v>
       </c>
       <c r="B89">
-        <v>3.6137827015131614</v>
+        <v>1.3478538778114693</v>
       </c>
       <c r="C89">
-        <v>0.84283222115128109</v>
+        <v>0.38139434061318156</v>
       </c>
       <c r="D89">
-        <v>-0.43520763014846237</v>
+        <v>3.5156730478015259</v>
       </c>
       <c r="E89">
-        <v>-0.67313838821150807</v>
+        <v>0.46855541743494672</v>
       </c>
       <c r="F89">
-        <v>-0.72993753170428322</v>
+        <v>0.57977206825760619</v>
       </c>
       <c r="G89">
-        <v>-0.68897022015062426</v>
+        <v>0.30648016076600687</v>
       </c>
       <c r="H89">
-        <v>-1.0670877889362724</v>
+        <v>0.17128645452943492</v>
       </c>
       <c r="I89">
-        <v>-1.1308121058275218</v>
+        <v>-1.0645346889563587</v>
       </c>
       <c r="J89">
-        <v>-1.0015247194761772</v>
+        <v>-0.30871754638322252</v>
       </c>
       <c r="K89">
-        <v>-0.56211543548732845</v>
+        <v>6.556885397645551E-2</v>
       </c>
       <c r="L89">
-        <v>-0.38833419101925221</v>
+        <v>-0.27175801828161245</v>
       </c>
       <c r="M89">
-        <v>-0.18113744425487122</v>
+        <v>-0.23366108666756749</v>
       </c>
       <c r="N89">
         <v>-0.5008439067958399</v>
@@ -7521,43 +8196,43 @@
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>3.8598961246113079</v>
+        <v>3.8454815215745546</v>
       </c>
       <c r="B90">
-        <v>-4.1923611297153203</v>
+        <v>2.1137526488450331</v>
       </c>
       <c r="C90">
-        <v>-5.0525676191137485</v>
+        <v>-0.7798390062073165</v>
       </c>
       <c r="D90">
-        <v>-2.5281664505675514</v>
+        <v>-0.1331344734162469</v>
       </c>
       <c r="E90">
-        <v>-2.0717496653916827</v>
+        <v>-0.1161635155594158</v>
       </c>
       <c r="F90">
-        <v>-1.2924377358850303</v>
+        <v>0.18135559268779852</v>
       </c>
       <c r="G90">
-        <v>-0.68414463679787807</v>
+        <v>2.1059375545036271E-2</v>
       </c>
       <c r="H90">
-        <v>-0.24097302396515499</v>
+        <v>-1.1703425096951062E-3</v>
       </c>
       <c r="I90">
-        <v>0.26837738536505662</v>
+        <v>-9.4694492007746947E-2</v>
       </c>
       <c r="J90">
-        <v>0.29490151692770894</v>
+        <v>-0.13371820597132877</v>
       </c>
       <c r="K90">
-        <v>-6.1095989915239422E-2</v>
+        <v>0.17162774632160979</v>
       </c>
       <c r="L90">
-        <v>-0.28417472435620894</v>
+        <v>9.4429047734299554E-2</v>
       </c>
       <c r="M90">
-        <v>-0.26369192472331604</v>
+        <v>-9.7054786969422865E-2</v>
       </c>
       <c r="N90">
         <v>-0.36212415618570482</v>

</xml_diff>